<commit_message>
renamed output tests 6.1 and 6.2
</commit_message>
<xml_diff>
--- a/testfiles/Tests.xlsx
+++ b/testfiles/Tests.xlsx
@@ -1,20 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech545_Spring2024/testfiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech545_Fall2024/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CA45819-3BB0-47B9-BC1E-E197CD5BD143}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD20353-2B92-440B-B207-A698BBA2655D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="DUMAC_ASSETCLASS_CASH">"Cash"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_COMMODITIES">"Commodities"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_FIXEDINCOME">"FixedIncome"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_GLOBALEQUITY">"GlobalEquity"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_HEDGEDSTRATEGIES">"HedgedStrategies"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_NATURALRESOURCES">"NaturalResources"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_OPPORTUNISTIC">"Opportunistic"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_PRIVATECAPITAL">"PrivateCapital"</definedName>
+    <definedName name="DUMAC_ASSETCLASS_REALESTATE">"RealEstate"</definedName>
+    <definedName name="DUMAC_INSTANCE_DAILY">"DAILY"</definedName>
+    <definedName name="DUMAC_INSTANCE_DAILY_AGG">"DAILY_AGG"</definedName>
+    <definedName name="DUMAC_INSTANCE_MONTHLY">"MONTHLY"</definedName>
+    <definedName name="DUMAC_INSTANCE_MONTHLY_AGG">"MONTHLY_AGG"</definedName>
+    <definedName name="DUMAC_INSTANCE_MONTHLY_AGG_FINAL">"MONTHLY_AGG_FINAL"</definedName>
+    <definedName name="DUMAC_POOL_ERP">"ERP"</definedName>
+    <definedName name="DUMAC_POOL_HSP">"HSP"</definedName>
+    <definedName name="DUMAC_POOL_LTP">"LTP"</definedName>
+    <definedName name="DUMAC_POOL_TDE">"TDE"</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -497,7 +517,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>